<commit_message>
PROD rec and logs
</commit_message>
<xml_diff>
--- a/PROD/logs/20250918/20250918_GMS_Trade_File_xgb_prod_12hr.xlsx
+++ b/PROD/logs/20250918/20250918_GMS_Trade_File_xgb_prod_12hr.xlsx
@@ -528,7 +528,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ADU5 Curncy</t>
+          <t>ADZ5 Curncy</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -660,7 +660,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>BPU5 Curncy</t>
+          <t>BPZ5 Curncy</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -671,7 +671,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -705,7 +705,7 @@
         <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>-14</v>
+        <v>14</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
@@ -737,7 +737,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -771,7 +771,7 @@
         <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>16</v>
+        <v>-16</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
@@ -803,7 +803,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -837,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
@@ -858,7 +858,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ESU5 Index</t>
+          <t>ESZ5 Index</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -924,7 +924,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ECU5 Curncy</t>
+          <t>ECZ5 Curncy</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -1056,7 +1056,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>JYU5 Curncy</t>
+          <t>JYZ5 Curncy</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1101,7 +1101,7 @@
         <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>-14</v>
+        <v>14</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
@@ -1122,7 +1122,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>NQU5 Index</t>
+          <t>NQZ5 Index</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -1133,7 +1133,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1167,7 +1167,7 @@
         <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>-6</v>
+        <v>6</v>
       </c>
       <c r="P11" t="inlineStr">
         <is>
@@ -1188,18 +1188,18 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>RTYU5 Index</t>
+          <t>RTYZ5 Index</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" t="n">
         <v>5</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1233,7 +1233,7 @@
         <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>-27</v>
+        <v>26</v>
       </c>
       <c r="P12" t="inlineStr">
         <is>
@@ -1456,7 +1456,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E16" t="n">
         <v>5</v>
@@ -1497,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="O16" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P16" t="inlineStr">
         <is>
@@ -1584,7 +1584,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>RXU5 Comdty</t>
+          <t>RXZ5 Comdty</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -1650,7 +1650,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>OEU5 Comdty</t>
+          <t>OZU5 Comdty</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -1716,7 +1716,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>CLV5 Comdty</t>
+          <t>CLZ5 Comdty</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1793,7 +1793,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1827,7 +1827,7 @@
         <v>0</v>
       </c>
       <c r="O21" t="n">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="P21" t="inlineStr">
         <is>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1893,7 +1893,7 @@
         <v>0</v>
       </c>
       <c r="O22" t="n">
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="P22" t="inlineStr">
         <is>
@@ -1914,7 +1914,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>NGV25 Comdty</t>
+          <t>NGX25 Comdty</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -2057,7 +2057,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -2091,7 +2091,7 @@
         <v>0</v>
       </c>
       <c r="O25" t="n">
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="P25" t="inlineStr">
         <is>

</xml_diff>